<commit_message>
2.1.0 Action specific timeouts.
</commit_message>
<xml_diff>
--- a/sample-tests.xlsx
+++ b/sample-tests.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="pwtest" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="68">
   <si>
     <t xml:space="preserve">Desc</t>
   </si>
@@ -50,52 +50,55 @@
     <t xml:space="preserve">url</t>
   </si>
   <si>
+    <t xml:space="preserve">title,10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Interne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Example</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(//a)[3]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add/Remove</t>
+  </si>
+  <si>
+    <t xml:space="preserve">click</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(//button)[1]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(//button)[2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exists:not</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Case 2</t>
+  </si>
+  <si>
     <t xml:space="preserve">title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Interne</t>
-  </si>
-  <si>
-    <t xml:space="preserve">h2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">assert</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Example</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(//a)[3]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Add/Remove</t>
-  </si>
-  <si>
-    <t xml:space="preserve">click</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Step 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">h3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(//button)[1]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Add</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(//button)[2]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">exists:not</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delete</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Case 2</t>
   </si>
   <si>
     <t xml:space="preserve">The Internet</t>
@@ -441,10 +444,10 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="bottomLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -618,26 +621,26 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D19" s="6" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>16</v>
@@ -654,34 +657,34 @@
         <v>12</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>16</v>
@@ -689,7 +692,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>11</v>
@@ -698,12 +701,12 @@
         <v>12</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>16</v>
@@ -711,7 +714,7 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>11</v>
@@ -720,7 +723,7 @@
         <v>12</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -728,7 +731,7 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -744,26 +747,26 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D35" s="6" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>16</v>
@@ -780,69 +783,69 @@
         <v>12</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="6"/>
       <c r="C40" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="6"/>
       <c r="C41" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C43" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E44" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -858,18 +861,18 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D48" s="6" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -883,57 +886,57 @@
         <v>12</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C52" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C53" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E53" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C54" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C55" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -949,23 +952,23 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D59" s="6" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C60" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D62" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="1048450" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1113,7 +1116,7 @@
   </sheetPr>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -1149,13 +1152,13 @@
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>8</v>
@@ -1164,15 +1167,15 @@
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D4" s="6" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D5" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E5" s="8" t="n">
         <v>1500</v>
@@ -1181,15 +1184,15 @@
     <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C6" s="6"/>
       <c r="D6" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2.2.1 Action dblclick and sleep. Logs colored.
</commit_message>
<xml_diff>
--- a/sample-tests.xlsx
+++ b/sample-tests.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="basic" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,6 +13,8 @@
     <sheet name="script" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="attrib_href" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="iframe" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="sleep" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="dblclick" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="110">
   <si>
     <t xml:space="preserve">Desc</t>
   </si>
@@ -312,6 +314,48 @@
   </si>
   <si>
     <t xml:space="preserve">Testersdock.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">action – sleep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://123timer.com/5-second</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123Timer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text=Start Pause &gt;&gt; nth=0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sleep,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">div.alertable-message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exists</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">action – dblclick</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://tecagile.com/double-click-test/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Online Double</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#darea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dblclick</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dummy</t>
   </si>
 </sst>
 </file>
@@ -1231,10 +1275,10 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.94"/>
@@ -1606,7 +1650,7 @@
       <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.69"/>
@@ -1685,11 +1729,11 @@
   </sheetPr>
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="9" width="12.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="9" width="10.36"/>
@@ -1826,4 +1870,378 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.33"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1"/>
+      <c r="B3" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1"/>
+      <c r="B3" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="E19" s="2"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
2.2.2 Quick regression fix in click.
</commit_message>
<xml_diff>
--- a/sample-tests.xlsx
+++ b/sample-tests.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="110">
   <si>
     <t xml:space="preserve">Desc</t>
   </si>
@@ -127,60 +127,63 @@
     <t xml:space="preserve">Case – timeout</t>
   </si>
   <si>
+    <t xml:space="preserve">https://the-internet.herokuapp.com/dynamic_controls</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(//h4)[1]</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dynamic Controls</t>
   </si>
   <si>
+    <t xml:space="preserve">p#message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assert,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enabled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Case – DnD TODO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(//a)[11]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">div#column-a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">div#column-b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dnd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assertx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Case – key</t>
+  </si>
+  <si>
+    <t xml:space="preserve">key</t>
+  </si>
+  <si>
     <t xml:space="preserve">click:text</t>
   </si>
   <si>
-    <t xml:space="preserve">(//h4)[1]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">p#message</t>
-  </si>
-  <si>
-    <t xml:space="preserve">assert,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">enabled</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Case – DnD TODO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(//a)[11]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Drag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">div#column-a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">div#column-b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dnd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">assertx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Case – key</t>
-  </si>
-  <si>
-    <t xml:space="preserve">key</t>
-  </si>
-  <si>
     <t xml:space="preserve">Key</t>
   </si>
   <si>
@@ -353,9 +356,6 @@
   </si>
   <si>
     <t xml:space="preserve">dblclick</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dummy</t>
   </si>
 </sst>
 </file>
@@ -586,14 +586,14 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E57" activeCellId="0" sqref="E57"/>
+      <selection pane="bottomLeft" activeCell="E50" activeCellId="0" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="41.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="46.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="21.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="6" style="1" width="12.43"/>
@@ -839,7 +839,7 @@
         <v>6</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>8</v>
@@ -847,65 +847,68 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>34</v>
+        <v>20</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D29" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="E28" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="6" t="s">
-        <v>39</v>
+      <c r="B31" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>7</v>
-      </c>
       <c r="D32" s="5" t="s">
-        <v>8</v>
+        <v>40</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D33" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>16</v>
+      <c r="C33" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -913,56 +916,56 @@
         <v>41</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E34" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C35" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="5" t="s">
-        <v>25</v>
-      </c>
+      <c r="B37" s="5"/>
       <c r="C37" s="1" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="5"/>
       <c r="C38" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C39" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D38" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="5"/>
-      <c r="C39" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="D39" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -970,163 +973,153 @@
         <v>43</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>48</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C41" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>48</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C42" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E42" s="2" t="s">
         <v>44</v>
       </c>
     </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="6" t="s">
-        <v>49</v>
+      <c r="B44" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>7</v>
-      </c>
       <c r="D45" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D46" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E46" s="7" t="s">
+      <c r="E45" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C47" s="1" t="s">
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C46" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D47" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="5" t="s">
+      <c r="D46" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="5" t="s">
         <v>25</v>
       </c>
+      <c r="C48" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="1" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D50" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C51" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E50" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C51" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="E51" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C52" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C53" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="6" t="s">
-        <v>57</v>
+      <c r="B55" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>7</v>
-      </c>
       <c r="D56" s="5" t="s">
-        <v>8</v>
+        <v>40</v>
+      </c>
+      <c r="E56" s="7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D57" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E57" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C58" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D60" s="1" t="s">
+      <c r="C57" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="D57" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D59" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048447" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048448" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048449" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048450" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1278,7 +1271,7 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.94"/>
@@ -1303,7 +1296,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1338,20 +1331,20 @@
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>24</v>
@@ -1377,40 +1370,40 @@
         <v>18</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>24</v>
@@ -1427,7 +1420,7 @@
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1"/>
       <c r="B13" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>17</v>
@@ -1436,14 +1429,14 @@
         <v>18</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>24</v>
@@ -1460,7 +1453,7 @@
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1"/>
       <c r="B16" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>17</v>
@@ -1469,7 +1462,7 @@
         <v>18</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1482,36 +1475,36 @@
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1"/>
       <c r="B18" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1"/>
       <c r="B19" s="5"/>
       <c r="C19" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1"/>
       <c r="B20" s="5"/>
       <c r="C20" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>24</v>
@@ -1528,7 +1521,7 @@
         <v>18</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1580,18 +1573,18 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>8</v>
@@ -1603,12 +1596,12 @@
         <v>40</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D5" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E5" s="8" t="n">
         <v>1500</v>
@@ -1617,15 +1610,15 @@
     <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1650,7 +1643,7 @@
       <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.69"/>
@@ -1733,7 +1726,7 @@
       <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="9" width="12.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="9" width="10.36"/>
@@ -1744,7 +1737,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B1" s="6"/>
     </row>
@@ -1753,7 +1746,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>8</v>
@@ -1761,41 +1754,41 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>86</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="1"/>
       <c r="D6" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="1"/>
       <c r="D7" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E7" s="10"/>
     </row>
@@ -1809,7 +1802,7 @@
         <v>25</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>8</v>
@@ -1817,48 +1810,48 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>18</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>18</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D14" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1883,7 +1876,7 @@
       <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.33"/>
@@ -1908,7 +1901,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1918,10 +1911,10 @@
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>8</v>
@@ -1936,14 +1929,14 @@
         <v>40</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>24</v>
@@ -1955,7 +1948,7 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E6" s="2"/>
     </row>
@@ -1963,7 +1956,7 @@
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>30</v>
@@ -1975,7 +1968,7 @@
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E8" s="2"/>
     </row>
@@ -1983,10 +1976,10 @@
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E9" s="2"/>
     </row>
@@ -1994,13 +1987,13 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>18</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2049,10 +2042,10 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.67"/>
@@ -2077,7 +2070,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2087,10 +2080,10 @@
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>8</v>
@@ -2105,14 +2098,14 @@
         <v>40</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>24</v>
@@ -2123,10 +2116,10 @@
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E6" s="2"/>
     </row>
@@ -2134,7 +2127,7 @@
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>18</v>
@@ -2147,7 +2140,7 @@
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>24</v>
@@ -2158,7 +2151,7 @@
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>18</v>
@@ -2171,10 +2164,10 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E10" s="2"/>
     </row>
@@ -2182,7 +2175,7 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>18</v>
@@ -2199,9 +2192,6 @@
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="0" t="s">
-        <v>109</v>
-      </c>
       <c r="E13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
2.4.0 Console output revamp.
</commit_message>
<xml_diff>
--- a/sample-tests.xlsx
+++ b/sample-tests.xlsx
@@ -13,10 +13,11 @@
     <sheet name="timeout" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="keys" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="script" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="attrib_href" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="attrib_href" sheetId="6" state="hidden" r:id="rId7"/>
     <sheet name="iframe" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="sleep" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="dblclick" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="file" sheetId="10" state="visible" r:id="rId11"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="137">
   <si>
     <t xml:space="preserve">Desc</t>
   </si>
@@ -48,6 +49,9 @@
     <t xml:space="preserve">Case – click</t>
   </si>
   <si>
+    <t xml:space="preserve">id 1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Step 1</t>
   </si>
   <si>
@@ -57,18 +61,27 @@
     <t xml:space="preserve">url</t>
   </si>
   <si>
+    <t xml:space="preserve">id 2</t>
+  </si>
+  <si>
     <t xml:space="preserve">title</t>
   </si>
   <si>
     <t xml:space="preserve">The Interne</t>
   </si>
   <si>
+    <t xml:space="preserve">id 3</t>
+  </si>
+  <si>
     <t xml:space="preserve">title:exact</t>
   </si>
   <si>
     <t xml:space="preserve">The Internet</t>
   </si>
   <si>
+    <t xml:space="preserve">id 4</t>
+  </si>
+  <si>
     <t xml:space="preserve">h2</t>
   </si>
   <si>
@@ -78,42 +91,93 @@
     <t xml:space="preserve">Example</t>
   </si>
   <si>
+    <t xml:space="preserve">id 5</t>
+  </si>
+  <si>
     <t xml:space="preserve">assert:exact</t>
   </si>
   <si>
     <t xml:space="preserve">Available Examples</t>
   </si>
   <si>
+    <t xml:space="preserve">id 6</t>
+  </si>
+  <si>
     <t xml:space="preserve">(//a)[3]</t>
   </si>
   <si>
     <t xml:space="preserve">Add/Remove</t>
   </si>
   <si>
+    <t xml:space="preserve">id 7</t>
+  </si>
+  <si>
     <t xml:space="preserve">click</t>
   </si>
   <si>
+    <t xml:space="preserve">id 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">print</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First of Basics done.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id 10</t>
+  </si>
+  <si>
     <t xml:space="preserve">Step 2</t>
   </si>
   <si>
     <t xml:space="preserve">h3</t>
   </si>
   <si>
+    <t xml:space="preserve">id 11</t>
+  </si>
+  <si>
     <t xml:space="preserve">(//button)[1]</t>
   </si>
   <si>
     <t xml:space="preserve">Add</t>
   </si>
   <si>
+    <t xml:space="preserve">id 12</t>
+  </si>
+  <si>
     <t xml:space="preserve">(//button)[2]</t>
   </si>
   <si>
     <t xml:space="preserve">exists:not</t>
   </si>
   <si>
+    <t xml:space="preserve">id 13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id 14</t>
+  </si>
+  <si>
     <t xml:space="preserve">Delete</t>
   </si>
   <si>
+    <t xml:space="preserve">id 15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id 16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id 17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Second of Basics done.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id 18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id 19</t>
+  </si>
+  <si>
     <t xml:space="preserve">end</t>
   </si>
   <si>
@@ -325,6 +389,57 @@
   </si>
   <si>
     <t xml:space="preserve">dblclick</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Action: file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://the-internet.herokuapp.com/upload</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#file-upload</t>
+  </si>
+  <si>
+    <t xml:space="preserve">file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/svr/Downloads/strawberry.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#file-submit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#uploaded-files</t>
+  </si>
+  <si>
+    <t xml:space="preserve">strawberry.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Case 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3schools.com/howto/tryit.asp?filename=tryhow_html_file_upload_button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tryit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#iframeResult</t>
+  </si>
+  <si>
+    <t xml:space="preserve">input[name="filename"]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">input[type="submit"]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Submitted Form Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//div[1]</t>
   </si>
 </sst>
 </file>
@@ -428,7 +543,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -470,6 +585,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -555,7 +674,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
+      <selection pane="bottomLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -591,153 +710,222 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6"/>
+      <c r="A3" s="6" t="s">
+        <v>6</v>
+      </c>
       <c r="B3" s="6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
+        <v>10</v>
+      </c>
       <c r="D4" s="6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="D5" s="6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="C7" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0"/>
+      <c r="A8" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="C8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="E8" s="2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="C9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="E12" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C13" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="C14" s="1" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6" t="s">
+        <v>40</v>
+      </c>
       <c r="C15" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="C16" s="1" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6" t="s">
+        <v>43</v>
+      </c>
       <c r="C17" s="1" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6" t="s">
+        <v>45</v>
+      </c>
       <c r="D19" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048407" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048408" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>29</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048409" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048410" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048411" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -917,6 +1105,210 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E30"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="78.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="44.43"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C7" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1"/>
+      <c r="B9" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D14" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -928,7 +1320,7 @@
       <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.45"/>
@@ -962,7 +1354,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -981,13 +1373,13 @@
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="1"/>
@@ -1005,10 +1397,10 @@
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -1024,10 +1416,10 @@
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="1"/>
@@ -1059,16 +1451,16 @@
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="6" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -1084,13 +1476,13 @@
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -1106,13 +1498,13 @@
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -1128,13 +1520,13 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -1150,13 +1542,13 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -1190,7 +1582,7 @@
       <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="46.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.68"/>
@@ -1225,7 +1617,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1244,13 +1636,13 @@
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="1"/>
@@ -1268,10 +1660,10 @@
       <c r="B4" s="6"/>
       <c r="C4" s="1"/>
       <c r="D4" s="6" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -1287,13 +1679,13 @@
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -1309,10 +1701,10 @@
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="1"/>
@@ -1329,13 +1721,13 @@
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -1366,7 +1758,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J23" activeCellId="0" sqref="J23"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1395,7 +1787,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1405,13 +1797,13 @@
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E3" s="2"/>
     </row>
@@ -1420,33 +1812,33 @@
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E6" s="2"/>
     </row>
@@ -1460,52 +1852,52 @@
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1"/>
       <c r="B8" s="6" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E11" s="2"/>
     </row>
@@ -1519,26 +1911,26 @@
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1"/>
       <c r="B13" s="6" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E14" s="2"/>
     </row>
@@ -1552,16 +1944,16 @@
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1"/>
       <c r="B16" s="6" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1574,39 +1966,39 @@
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1"/>
       <c r="B18" s="6" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1"/>
       <c r="B19" s="6"/>
       <c r="C19" s="1" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1"/>
       <c r="B20" s="6"/>
       <c r="C20" s="1" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E20" s="2"/>
     </row>
@@ -1614,13 +2006,13 @@
       <c r="A21" s="1"/>
       <c r="B21" s="6"/>
       <c r="C21" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1672,35 +2064,35 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D4" s="6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>64</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D5" s="6" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
       <c r="E5" s="8" t="n">
         <v>1500</v>
@@ -1709,15 +2101,15 @@
     <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C6" s="6"/>
       <c r="D6" s="6" t="s">
-        <v>66</v>
+        <v>87</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1776,29 +2168,29 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>69</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1822,7 +2214,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
+      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1836,58 +2228,58 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="B1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="0" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
-        <v>76</v>
+        <v>97</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="1" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="1"/>
       <c r="D6" s="6" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="1"/>
       <c r="D7" s="6" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="E7" s="10"/>
     </row>
@@ -1898,59 +2290,59 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="9" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>81</v>
+        <v>102</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>85</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>85</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D14" s="6" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1975,7 +2367,7 @@
       <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.33"/>
@@ -2000,7 +2392,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>86</v>
+        <v>107</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2010,13 +2402,13 @@
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="6" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E3" s="2"/>
     </row>
@@ -2025,20 +2417,20 @@
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>88</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>89</v>
+        <v>110</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E5" s="2"/>
     </row>
@@ -2047,7 +2439,7 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>90</v>
+        <v>111</v>
       </c>
       <c r="E6" s="2"/>
     </row>
@@ -2055,10 +2447,10 @@
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>91</v>
+        <v>112</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="E7" s="2"/>
     </row>
@@ -2067,7 +2459,7 @@
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>90</v>
+        <v>111</v>
       </c>
       <c r="E8" s="2"/>
     </row>
@@ -2075,10 +2467,10 @@
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>91</v>
+        <v>112</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>92</v>
+        <v>113</v>
       </c>
       <c r="E9" s="2"/>
     </row>
@@ -2086,13 +2478,13 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>91</v>
+        <v>112</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>93</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2144,7 +2536,7 @@
       <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.67"/>
@@ -2169,7 +2561,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>94</v>
+        <v>115</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2179,13 +2571,13 @@
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="6" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E3" s="2"/>
     </row>
@@ -2194,20 +2586,20 @@
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>96</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>97</v>
+        <v>118</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E5" s="2"/>
     </row>
@@ -2215,10 +2607,10 @@
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>97</v>
+        <v>118</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>98</v>
+        <v>119</v>
       </c>
       <c r="E6" s="2"/>
     </row>
@@ -2226,10 +2618,10 @@
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>97</v>
+        <v>118</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E7" s="2" t="n">
         <v>1</v>
@@ -2239,10 +2631,10 @@
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>97</v>
+        <v>118</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E8" s="2"/>
     </row>
@@ -2250,10 +2642,10 @@
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>97</v>
+        <v>118</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E9" s="2" t="n">
         <v>1</v>
@@ -2263,10 +2655,10 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>97</v>
+        <v>118</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>98</v>
+        <v>119</v>
       </c>
       <c r="E10" s="2"/>
     </row>
@@ -2274,10 +2666,10 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>97</v>
+        <v>118</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E11" s="2" t="n">
         <v>2</v>

</xml_diff>

<commit_message>
2.4.1 Pause works in --headed mode.
</commit_message>
<xml_diff>
--- a/sample-tests.xlsx
+++ b/sample-tests.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="basics" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,11 +13,12 @@
     <sheet name="timeout" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="keys" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="script" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="attrib_href" sheetId="6" state="hidden" r:id="rId7"/>
+    <sheet name="attrib_href" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="iframe" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="sleep" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="dblclick" sheetId="9" state="visible" r:id="rId10"/>
     <sheet name="file" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="pause" sheetId="11" state="visible" r:id="rId12"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="141">
   <si>
     <t xml:space="preserve">Desc</t>
   </si>
@@ -440,6 +441,18 @@
   </si>
   <si>
     <t xml:space="preserve">//div[1]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">action – pause and print</t>
+  </si>
+  <si>
+    <t xml:space="preserve">line before pause</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pause</t>
+  </si>
+  <si>
+    <t xml:space="preserve">line after pause</t>
   </si>
 </sst>
 </file>
@@ -671,7 +684,7 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
@@ -1116,7 +1129,7 @@
       <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="78.39"/>
@@ -1309,6 +1322,142 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.2"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1"/>
+      <c r="B3" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="E11" s="2"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -1320,7 +1469,7 @@
       <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.45"/>
@@ -1582,7 +1731,7 @@
       <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="46.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.68"/>
@@ -2034,7 +2183,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2533,7 +2682,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
2.4.2 Some console log refactoring.
</commit_message>
<xml_diff>
--- a/sample-tests.xlsx
+++ b/sample-tests.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="basics" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,6 +19,8 @@
     <sheet name="dblclick" sheetId="9" state="visible" r:id="rId10"/>
     <sheet name="file" sheetId="10" state="visible" r:id="rId11"/>
     <sheet name="pause" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="if_endif" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="loop" sheetId="13" state="visible" r:id="rId14"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="158">
   <si>
     <t xml:space="preserve">Desc</t>
   </si>
@@ -251,13 +253,22 @@
     <t xml:space="preserve">keys</t>
   </si>
   <si>
+    <t xml:space="preserve">tomsmith*9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">input#password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SuperSecretPassword!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sleep,3</t>
+  </si>
+  <si>
     <t xml:space="preserve">tomsmith</t>
   </si>
   <si>
-    <t xml:space="preserve">input#password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SuperSecretPassword!</t>
+    <t xml:space="preserve">fills replaces the whole text</t>
   </si>
   <si>
     <t xml:space="preserve">button.radius</t>
@@ -365,9 +376,6 @@
     <t xml:space="preserve">text=Start Pause &gt;&gt; nth=0</t>
   </si>
   <si>
-    <t xml:space="preserve">sleep,3</t>
-  </si>
-  <si>
     <t xml:space="preserve">div.alertable-message</t>
   </si>
   <si>
@@ -443,16 +451,61 @@
     <t xml:space="preserve">//div[1]</t>
   </si>
   <si>
-    <t xml:space="preserve">action – pause and print</t>
-  </si>
-  <si>
-    <t xml:space="preserve">line before pause</t>
-  </si>
-  <si>
     <t xml:space="preserve">pause</t>
   </si>
   <si>
-    <t xml:space="preserve">line after pause</t>
+    <t xml:space="preserve">action – if endif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">try 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://demoqa.com/radio-button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ToolsQA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//span[@class='text-success']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assert?miss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Impressive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if</t>
+  </si>
+  <si>
+    <t xml:space="preserve">miss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Impressive not there!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">endif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">----</t>
+  </si>
+  <si>
+    <t xml:space="preserve">try 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assert?nope</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nope</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//label[contains(.,'Impressive')]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inside if</t>
+  </si>
+  <si>
+    <t xml:space="preserve">outside if</t>
   </si>
 </sst>
 </file>
@@ -556,7 +609,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -603,6 +656,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1129,7 +1186,7 @@
       <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="78.39"/>
@@ -1156,7 +1213,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1165,10 +1222,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>9</v>
@@ -1187,18 +1244,18 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>27</v>
@@ -1206,22 +1263,22 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>18</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1"/>
       <c r="B9" s="6" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>9</v>
@@ -1233,32 +1290,32 @@
         <v>11</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E11" s="7"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>27</v>
@@ -1266,37 +1323,37 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D14" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>18</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>18</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1327,13 +1384,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.61"/>
@@ -1359,7 +1416,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>137</v>
+        <v>67</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1369,10 +1426,10 @@
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="6" t="s">
-        <v>82</v>
+        <v>7</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>116</v>
+        <v>8</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>9</v>
@@ -1387,26 +1444,30 @@
         <v>11</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>117</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="0" t="s">
-        <v>29</v>
+      <c r="C5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>138</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="D6" s="1" t="s">
-        <v>139</v>
+        <v>27</v>
       </c>
       <c r="E6" s="2"/>
     </row>
@@ -1414,40 +1475,515 @@
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>140</v>
-      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="2"/>
+      <c r="B8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+      <c r="B9" s="6"/>
       <c r="C9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>139</v>
+      </c>
       <c r="E9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="2"/>
+      <c r="C10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1"/>
+      <c r="B14" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1"/>
+      <c r="B17" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1"/>
+      <c r="B19" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E1048576"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="52.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.55"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="12"/>
+      <c r="B3" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="12"/>
+      <c r="C4" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="12"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="12"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="12"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="12"/>
+      <c r="B8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="12"/>
+      <c r="B9" s="1"/>
+      <c r="D9" s="0" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="12"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="12"/>
+      <c r="B11" s="1"/>
       <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
       <c r="E11" s="2"/>
     </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="12"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="12"/>
+      <c r="B13" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="12"/>
+      <c r="C14" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="12"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="12"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="D21" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="D22" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="D23" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="7"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="2"/>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1904,10 +2440,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2042,72 +2578,75 @@
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="1"/>
+      <c r="D11" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="E11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
+      <c r="C12" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1"/>
-      <c r="B13" s="6" t="s">
-        <v>77</v>
-      </c>
+      <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>17</v>
+        <v>79</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>78</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
-      <c r="C14" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
       <c r="E14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="2"/>
+      <c r="B15" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1"/>
-      <c r="B16" s="6" t="s">
-        <v>80</v>
-      </c>
+      <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>17</v>
+        <v>82</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>70</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="E16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1"/>
-      <c r="B17" s="6"/>
+      <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
@@ -2115,53 +2654,75 @@
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1"/>
       <c r="B18" s="6" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>71</v>
+        <v>17</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>72</v>
+        <v>18</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1"/>
       <c r="B19" s="6"/>
-      <c r="C19" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>75</v>
-      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1"/>
-      <c r="B20" s="6"/>
+      <c r="B20" s="6" t="s">
+        <v>84</v>
+      </c>
       <c r="C20" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E20" s="2"/>
+        <v>72</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1"/>
       <c r="B21" s="6"/>
       <c r="C21" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>78</v>
+      <c r="E23" s="2" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -2213,18 +2774,18 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>9</v>
@@ -2236,12 +2797,12 @@
         <v>11</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D5" s="6" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="E5" s="8" t="n">
         <v>1500</v>
@@ -2250,15 +2811,15 @@
     <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C6" s="6"/>
       <c r="D6" s="6" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -2317,7 +2878,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2333,13 +2894,13 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2377,7 +2938,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B1" s="5"/>
     </row>
@@ -2386,7 +2947,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>9</v>
@@ -2394,41 +2955,41 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="1"/>
       <c r="D6" s="6" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="1"/>
       <c r="D7" s="6" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E7" s="10"/>
     </row>
@@ -2442,7 +3003,7 @@
         <v>32</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>9</v>
@@ -2450,48 +3011,48 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>18</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>72</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>18</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D14" s="6" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2541,7 +3102,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2551,10 +3112,10 @@
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="6" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>9</v>
@@ -2569,14 +3130,14 @@
         <v>11</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>27</v>
@@ -2588,7 +3149,7 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>111</v>
+        <v>76</v>
       </c>
       <c r="E6" s="2"/>
     </row>
@@ -2596,7 +3157,7 @@
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>39</v>
@@ -2608,7 +3169,7 @@
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>111</v>
+        <v>76</v>
       </c>
       <c r="E8" s="2"/>
     </row>
@@ -2616,10 +3177,10 @@
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E9" s="2"/>
     </row>
@@ -2627,13 +3188,13 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>18</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2682,7 +3243,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2710,7 +3271,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2720,10 +3281,10 @@
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="6" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>9</v>
@@ -2738,14 +3299,14 @@
         <v>11</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>27</v>
@@ -2756,10 +3317,10 @@
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E6" s="2"/>
     </row>
@@ -2767,7 +3328,7 @@
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>18</v>
@@ -2780,7 +3341,7 @@
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>27</v>
@@ -2791,7 +3352,7 @@
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>18</v>
@@ -2804,10 +3365,10 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E10" s="2"/>
     </row>
@@ -2815,7 +3376,7 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
2.5.0 Action: if endif works!
</commit_message>
<xml_diff>
--- a/sample-tests.xlsx
+++ b/sample-tests.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="159">
   <si>
     <t xml:space="preserve">Desc</t>
   </si>
@@ -493,19 +493,22 @@
     <t xml:space="preserve">try 2</t>
   </si>
   <si>
+    <t xml:space="preserve">//label[contains(.,'Impressive')]</t>
+  </si>
+  <si>
     <t xml:space="preserve">assert?nope</t>
   </si>
   <si>
     <t xml:space="preserve">nope</t>
   </si>
   <si>
-    <t xml:space="preserve">//label[contains(.,'Impressive')]</t>
-  </si>
-  <si>
     <t xml:space="preserve">inside if</t>
   </si>
   <si>
     <t xml:space="preserve">outside if</t>
+  </si>
+  <si>
+    <t xml:space="preserve">try 3</t>
   </si>
 </sst>
 </file>
@@ -1672,10 +1675,10 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
+      <selection pane="topLeft" activeCell="M12" activeCellId="0" sqref="M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="52.48"/>
@@ -1839,74 +1842,75 @@
       <c r="A16" s="12"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="7"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="12"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="E16" s="0" t="s">
+      <c r="D17" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E17" s="0" t="s">
         <v>146</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="1"/>
+      <c r="D18" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E18" s="0" t="s">
         <v>155</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>146</v>
+        <v>153</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="0" t="s">
-        <v>29</v>
+      <c r="C20" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
-      <c r="D21" s="1" t="s">
-        <v>150</v>
+      <c r="C21" s="1"/>
+      <c r="D21" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
-      <c r="D22" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>157</v>
+      <c r="D22" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1916,48 +1920,128 @@
         <v>29</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
+      <c r="D24" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
+      <c r="B26" s="6" t="s">
+        <v>158</v>
+      </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="7"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="2"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
+      <c r="C27" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="E27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="2"/>
+      <c r="D28" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="2"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="2"/>
+      <c r="D30" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="1"/>
+      <c r="C31" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="1"/>
+      <c r="C32" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="1"/>
+      <c r="D34" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="1"/>
+      <c r="D35" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="1"/>
+      <c r="D36" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -1982,7 +2066,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
2.5.1 if with negation. endif events.
</commit_message>
<xml_diff>
--- a/sample-tests.xlsx
+++ b/sample-tests.xlsx
@@ -20,7 +20,6 @@
     <sheet name="file" sheetId="10" state="visible" r:id="rId11"/>
     <sheet name="pause" sheetId="11" state="visible" r:id="rId12"/>
     <sheet name="if_endif" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="loop" sheetId="13" state="visible" r:id="rId14"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="162">
   <si>
     <t xml:space="preserve">Desc</t>
   </si>
@@ -478,16 +477,19 @@
     <t xml:space="preserve">if</t>
   </si>
   <si>
+    <t xml:space="preserve">!miss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Impressive is here!!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">endif</t>
+  </si>
+  <si>
     <t xml:space="preserve">miss</t>
   </si>
   <si>
-    <t xml:space="preserve">Impressive not there!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">endif</t>
-  </si>
-  <si>
-    <t xml:space="preserve">----</t>
+    <t xml:space="preserve">Impressive not there.</t>
   </si>
   <si>
     <t xml:space="preserve">try 2</t>
@@ -497,6 +499,12 @@
   </si>
   <si>
     <t xml:space="preserve">assert?nope</t>
+  </si>
+  <si>
+    <t xml:space="preserve">!nope</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All is fine</t>
   </si>
   <si>
     <t xml:space="preserve">nope</t>
@@ -1672,18 +1680,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1048576"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M12" activeCellId="0" sqref="M12"/>
+      <selection pane="topLeft" activeCell="I28" activeCellId="0" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="52.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1769,6 +1777,7 @@
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="12"/>
       <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
         <v>29</v>
       </c>
@@ -1779,6 +1788,7 @@
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="12"/>
       <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
       <c r="D9" s="0" t="s">
         <v>150</v>
       </c>
@@ -1787,287 +1797,346 @@
       <c r="A10" s="12"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="2" t="s">
+      <c r="D10" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="E10" s="0" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="12"/>
       <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
+      <c r="D11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="12"/>
       <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
+      <c r="D12" s="0" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="12"/>
-      <c r="B13" s="6" t="s">
-        <v>152</v>
-      </c>
+      <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="E13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="12"/>
-      <c r="C14" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>9</v>
-      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
       <c r="E14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="12"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>143</v>
-      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="12"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1" t="s">
+      <c r="B16" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="D16" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" s="7"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="12"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>146</v>
-      </c>
+      <c r="C17" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1"/>
+      <c r="A18" s="12"/>
+      <c r="B18" s="1"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>155</v>
+      <c r="D18" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1"/>
+      <c r="A19" s="12"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>27</v>
       </c>
+      <c r="E19" s="7"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1"/>
+      <c r="A20" s="12"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
         <v>144</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>18</v>
+        <v>155</v>
       </c>
       <c r="E20" s="0" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1"/>
+      <c r="A21" s="12"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="0" t="s">
-        <v>29</v>
+      <c r="D21" s="1" t="s">
+        <v>147</v>
       </c>
       <c r="E21" s="0" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1"/>
+      <c r="A22" s="12"/>
       <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="12"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1" t="s">
         <v>150</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="D23" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="D24" s="0" t="s">
-        <v>29</v>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1" t="s">
+        <v>147</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
+      <c r="C25" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1"/>
-      <c r="B26" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="2"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1"/>
-      <c r="C27" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="2"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="D29" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="D30" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1"/>
+      <c r="B32" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1"/>
+      <c r="C33" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="2"/>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E28" s="7" t="s">
+      <c r="E34" s="7" t="s">
         <v>143</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="1"/>
-      <c r="C29" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="E29" s="0" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="1"/>
-      <c r="D30" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E30" s="0" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="1"/>
-      <c r="C31" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D31" s="0" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="1"/>
-      <c r="C32" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E32" s="0" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="E33" s="0" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="1"/>
-      <c r="D34" s="1" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="1"/>
-      <c r="D35" s="0" t="s">
-        <v>29</v>
+      <c r="C35" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>155</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="1"/>
-      <c r="D36" s="0" t="s">
+      <c r="C36" s="1"/>
+      <c r="D36" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E36" s="0" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="E37" s="0" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C39" s="1"/>
+      <c r="D39" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="1"/>
+      <c r="C40" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="1"/>
+      <c r="C41" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="1"/>
+      <c r="D43" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="1"/>
+      <c r="D44" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="1"/>
+      <c r="D45" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
2.6.0 Select single or multiple options.
</commit_message>
<xml_diff>
--- a/sample-tests.xlsx
+++ b/sample-tests.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="basics" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,6 +20,7 @@
     <sheet name="file" sheetId="10" state="visible" r:id="rId11"/>
     <sheet name="pause" sheetId="11" state="visible" r:id="rId12"/>
     <sheet name="if_endif" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="select" sheetId="13" state="visible" r:id="rId14"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="172">
   <si>
     <t xml:space="preserve">Desc</t>
   </si>
@@ -517,6 +518,36 @@
   </si>
   <si>
     <t xml:space="preserve">try 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">action – select</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://letcode.in/dropdowns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LetCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#superheros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aq,ta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//p[@class='subtitle']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aquaman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avengers</t>
   </si>
 </sst>
 </file>
@@ -1682,8 +1713,8 @@
   </sheetPr>
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I28" activeCellId="0" sqref="I28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2136,6 +2167,142 @@
         <v>29</v>
       </c>
     </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K28" activeCellId="0" sqref="K28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.02"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="12"/>
+      <c r="B3" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="12"/>
+      <c r="C4" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="12"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C7" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D10" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
2.7.0 Tab catch, go in and out recursively.
</commit_message>
<xml_diff>
--- a/sample-tests.xlsx
+++ b/sample-tests.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="12"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="basics" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,6 +21,7 @@
     <sheet name="pause" sheetId="11" state="visible" r:id="rId12"/>
     <sheet name="if_endif" sheetId="12" state="visible" r:id="rId13"/>
     <sheet name="select" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="tab" sheetId="14" state="visible" r:id="rId15"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="182">
   <si>
     <t xml:space="preserve">Desc</t>
   </si>
@@ -548,6 +549,36 @@
   </si>
   <si>
     <t xml:space="preserve">Avengers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sheet – action – tab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://letcode.in/windows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Window</t>
+  </si>
+  <si>
+    <t xml:space="preserve">button#home</t>
+  </si>
+  <si>
+    <t xml:space="preserve">click:tab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing Hub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//a[@title='Koushik Chatterjee']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LinkedIn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tab:back</t>
+  </si>
+  <si>
+    <t xml:space="preserve">title?</t>
   </si>
 </sst>
 </file>
@@ -2185,11 +2216,11 @@
   </sheetPr>
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K28" activeCellId="0" sqref="K28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.66"/>
@@ -2303,6 +2334,135 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J18" activeCellId="0" sqref="J18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="35.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.09"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C3" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="1"/>
+      <c r="D4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C7" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D8" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D9" s="0" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D10" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D11" s="0" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D12" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
2.10.0 var action + fresh output.log on every run.
</commit_message>
<xml_diff>
--- a/sample-tests.xlsx
+++ b/sample-tests.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="13"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="basics" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,6 +22,7 @@
     <sheet name="if_endif" sheetId="12" state="visible" r:id="rId13"/>
     <sheet name="select" sheetId="13" state="visible" r:id="rId14"/>
     <sheet name="tab" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="var_set" sheetId="15" state="visible" r:id="rId16"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="194">
   <si>
     <t xml:space="preserve">Desc</t>
   </si>
@@ -579,6 +580,42 @@
   </si>
   <si>
     <t xml:space="preserve">title?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sheet - action - var</t>
+  </si>
+  <si>
+    <t xml:space="preserve">button#multi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">var</t>
+  </si>
+  <si>
+    <t xml:space="preserve">myvar1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">something</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xx{{myvar1}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">multi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">var:set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">myvar2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{myvar2}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">button#{{myvar2}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muiltiple windows</t>
   </si>
 </sst>
 </file>
@@ -2220,7 +2257,7 @@
       <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.66"/>
@@ -2352,11 +2389,11 @@
   </sheetPr>
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J18" activeCellId="0" sqref="J18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="35.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.02"/>
@@ -2463,6 +2500,140 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E24"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="37.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.86"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="1"/>
+      <c r="D5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D7" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D8" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D10" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
2.11.0 {{var}} takes from .env file if not local.
</commit_message>
<xml_diff>
--- a/sample-tests.xlsx
+++ b/sample-tests.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="196">
   <si>
     <t xml:space="preserve">Desc</t>
   </si>
@@ -616,6 +616,12 @@
   </si>
   <si>
     <t xml:space="preserve">Muiltiple windows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">try 2 - from .env</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{MYVAR}}</t>
   </si>
 </sst>
 </file>
@@ -2393,7 +2399,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="35.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.02"/>
@@ -2519,12 +2525,12 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="37.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.98"/>
@@ -2631,6 +2637,19 @@
       </c>
       <c r="E11" s="0" t="s">
         <v>193</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D14" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
2.13.0 assert value. clarify non-regex escape.
</commit_message>
<xml_diff>
--- a/sample-tests.xlsx
+++ b/sample-tests.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="14"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="basics" sheetId="1" state="visible" r:id="rId2"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="211">
   <si>
     <t xml:space="preserve">Desc</t>
   </si>
@@ -114,6 +114,21 @@
     <t xml:space="preserve">Add/Remove</t>
   </si>
   <si>
+    <t xml:space="preserve">(//div[@id='content']//li)[3]/a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basic Auth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">colon (:) works</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(//div[@id='content']//li)[3]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basic Auth (user and pass: admin)</t>
+  </si>
+  <si>
     <t xml:space="preserve">id 7</t>
   </si>
   <si>
@@ -183,6 +198,42 @@
     <t xml:space="preserve">id 19</t>
   </si>
   <si>
+    <t xml:space="preserve">step 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://demoqa.com/text-box</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ToolsQA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">input#userName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">keys</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tom*9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">input#userEmail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xyz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assert:value:exact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assert:value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m\*9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sleep,5</t>
+  </si>
+  <si>
     <t xml:space="preserve">end</t>
   </si>
   <si>
@@ -252,9 +303,6 @@
     <t xml:space="preserve">input#username</t>
   </si>
   <si>
-    <t xml:space="preserve">keys</t>
-  </si>
-  <si>
     <t xml:space="preserve">tomsmith*9</t>
   </si>
   <si>
@@ -463,9 +511,6 @@
   </si>
   <si>
     <t xml:space="preserve">https://demoqa.com/radio-button</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ToolsQA</t>
   </si>
   <si>
     <t xml:space="preserve">//span[@class='text-success']</t>
@@ -632,7 +677,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -654,6 +699,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -725,7 +776,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -756,6 +807,10 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -855,12 +910,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1048576"/>
+  <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
+      <selection pane="bottomLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -869,8 +924,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="46.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="21.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="6" style="1" width="12.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="32.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="7" style="1" width="12.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -974,149 +1030,239 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="6"/>
+      <c r="C9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="D9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="6"/>
+      <c r="B10" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="C10" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="D10" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="F10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6"/>
+      <c r="A11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>36</v>
-      </c>
+      <c r="A13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>37</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>38</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>39</v>
+        <v>18</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="D15" s="1" t="s">
-        <v>27</v>
+        <v>18</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>39</v>
+        <v>18</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>45</v>
+        <v>48</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048409" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048410" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048411" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048412" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>34</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D24" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C25" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C26" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C27" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C28" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D29" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D36" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
     <row r="1048414" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048415" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048416" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1282,8 +1428,8 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1329,7 +1475,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1338,10 +1484,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>123</v>
+        <v>139</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>9</v>
@@ -1360,41 +1506,41 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="0" t="s">
-        <v>124</v>
+        <v>140</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>125</v>
+        <v>141</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>126</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
-        <v>127</v>
+        <v>143</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="11" t="s">
-        <v>129</v>
+      <c r="E7" s="12" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1"/>
       <c r="B9" s="6" t="s">
-        <v>130</v>
+        <v>146</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>131</v>
+        <v>147</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>9</v>
@@ -1406,70 +1552,70 @@
         <v>11</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>133</v>
+        <v>149</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="E11" s="7"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>134</v>
+        <v>150</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>125</v>
+        <v>141</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>126</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>135</v>
+        <v>151</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D14" s="0" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
-        <v>133</v>
+        <v>149</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="0" t="s">
-        <v>136</v>
+        <v>152</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>18</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>137</v>
+        <v>153</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="0" t="s">
-        <v>138</v>
+        <v>154</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>18</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1487,7 +1633,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1532,7 +1678,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1567,23 +1713,23 @@
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E6" s="2"/>
     </row>
@@ -1597,7 +1743,7 @@
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1"/>
       <c r="B8" s="6" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>17</v>
@@ -1606,7 +1752,7 @@
         <v>18</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1614,7 +1760,7 @@
       <c r="B9" s="6"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>139</v>
+        <v>155</v>
       </c>
       <c r="E9" s="2"/>
     </row>
@@ -1622,36 +1768,36 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E12" s="2"/>
     </row>
@@ -1665,7 +1811,7 @@
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1"/>
       <c r="B14" s="6" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>17</v>
@@ -1674,17 +1820,17 @@
         <v>18</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E15" s="2"/>
     </row>
@@ -1698,7 +1844,7 @@
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1"/>
       <c r="B17" s="6" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>17</v>
@@ -1707,7 +1853,7 @@
         <v>18</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1720,39 +1866,39 @@
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1"/>
       <c r="B19" s="6" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1"/>
       <c r="B20" s="6"/>
       <c r="C20" s="1" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1"/>
       <c r="B21" s="6"/>
       <c r="C21" s="1" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E21" s="2"/>
     </row>
@@ -1766,13 +1912,13 @@
         <v>18</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1788,7 +1934,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1817,8 +1963,8 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
-        <v>140</v>
+      <c r="A2" s="13" t="s">
+        <v>156</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1826,18 +1972,18 @@
       <c r="E2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12"/>
+      <c r="A3" s="13"/>
       <c r="B3" s="6" t="s">
-        <v>141</v>
+        <v>157</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12"/>
+      <c r="A4" s="13"/>
       <c r="C4" s="6" t="s">
-        <v>142</v>
+        <v>158</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>9</v>
@@ -1845,123 +1991,123 @@
       <c r="E4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12"/>
+      <c r="A5" s="13"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>143</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>144</v>
+        <v>159</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>145</v>
+        <v>160</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>146</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="0" t="s">
-        <v>147</v>
+        <v>162</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>148</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="12"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>149</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="0" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="12"/>
+      <c r="A10" s="13"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="0" t="s">
-        <v>147</v>
+        <v>162</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>151</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="12"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>152</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="12"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="1"/>
       <c r="D12" s="0" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="12"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="E13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="12"/>
+      <c r="A14" s="13"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="12"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="12"/>
+      <c r="A16" s="13"/>
       <c r="B16" s="6" t="s">
-        <v>153</v>
+        <v>168</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="12"/>
+      <c r="A17" s="13"/>
       <c r="C17" s="6" t="s">
-        <v>142</v>
+        <v>158</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>9</v>
@@ -1969,101 +2115,101 @@
       <c r="E17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="12"/>
+      <c r="A18" s="13"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>143</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="12"/>
+      <c r="A19" s="13"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>154</v>
+        <v>169</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E19" s="7"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="12"/>
+      <c r="A20" s="13"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>144</v>
+        <v>159</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>146</v>
+        <v>161</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="12"/>
+      <c r="A21" s="13"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
-        <v>147</v>
+        <v>162</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="12"/>
+      <c r="A22" s="13"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>157</v>
+        <v>172</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="12"/>
+      <c r="A23" s="13"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1" t="s">
-        <v>147</v>
+        <v>162</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>158</v>
+        <v>173</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
-        <v>154</v>
+        <v>169</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
-        <v>144</v>
+        <v>159</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>146</v>
+        <v>161</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2071,37 +2217,37 @@
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="0" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>159</v>
+        <v>174</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="D28" s="1" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>158</v>
+        <v>173</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="D29" s="0" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>160</v>
+        <v>175</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="D30" s="0" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2111,7 +2257,7 @@
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1"/>
       <c r="B32" s="6" t="s">
-        <v>161</v>
+        <v>176</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -2120,7 +2266,7 @@
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1"/>
       <c r="C33" s="6" t="s">
-        <v>142</v>
+        <v>158</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>9</v>
@@ -2135,116 +2281,116 @@
         <v>11</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>143</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="1"/>
       <c r="C35" s="1" t="s">
-        <v>144</v>
+        <v>159</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>146</v>
+        <v>161</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1" t="s">
-        <v>147</v>
+        <v>162</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>157</v>
+        <v>172</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="1"/>
       <c r="D39" s="1" t="s">
-        <v>147</v>
+        <v>162</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>158</v>
+        <v>173</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="1"/>
       <c r="C40" s="1" t="s">
-        <v>154</v>
+        <v>169</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="1"/>
       <c r="C41" s="1" t="s">
-        <v>144</v>
+        <v>159</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>146</v>
+        <v>161</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="0" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>159</v>
+        <v>174</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="1"/>
       <c r="D43" s="1" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>158</v>
+        <v>173</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="1"/>
       <c r="D44" s="0" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>160</v>
+        <v>175</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="1"/>
       <c r="D45" s="0" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2288,8 +2434,8 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
-        <v>162</v>
+      <c r="A2" s="13" t="s">
+        <v>177</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2297,18 +2443,18 @@
       <c r="E2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12"/>
+      <c r="A3" s="13"/>
       <c r="B3" s="6" t="s">
-        <v>141</v>
+        <v>157</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12"/>
+      <c r="A4" s="13"/>
       <c r="C4" s="6" t="s">
-        <v>163</v>
+        <v>178</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>9</v>
@@ -2316,63 +2462,63 @@
       <c r="E4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12"/>
+      <c r="A5" s="13"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>164</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
-        <v>165</v>
+        <v>180</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>166</v>
+        <v>181</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>167</v>
+        <v>182</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
-        <v>168</v>
+        <v>183</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>18</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>169</v>
+        <v>184</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
-        <v>165</v>
+        <v>180</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>166</v>
+        <v>181</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>170</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>168</v>
+        <v>183</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>18</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>171</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D10" s="0" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2380,7 +2526,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2425,12 +2571,12 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>172</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="6" t="s">
-        <v>173</v>
+        <v>188</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>9</v>
@@ -2443,15 +2589,15 @@
         <v>11</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>174</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="0" t="s">
-        <v>175</v>
+        <v>190</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>176</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2459,15 +2605,15 @@
         <v>11</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>177</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
-        <v>178</v>
+        <v>193</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>176</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2475,12 +2621,12 @@
         <v>11</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>179</v>
+        <v>194</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="0" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2488,20 +2634,20 @@
         <v>11</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>177</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D11" s="0" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="6" t="s">
-        <v>181</v>
+        <v>196</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>174</v>
+        <v>189</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2509,7 +2655,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2524,11 +2670,11 @@
   </sheetPr>
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.77"/>
@@ -2556,17 +2702,17 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>182</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>141</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="6" t="s">
-        <v>173</v>
+        <v>188</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>9</v>
@@ -2579,84 +2725,84 @@
         <v>11</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>174</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
-        <v>183</v>
+        <v>198</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>184</v>
+        <v>199</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="0" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>186</v>
+        <v>201</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="0" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>187</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>188</v>
+        <v>203</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>189</v>
+        <v>204</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>190</v>
+        <v>205</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D10" s="0" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>191</v>
+        <v>206</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>192</v>
+        <v>207</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>18</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>194</v>
+        <v>209</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D14" s="0" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>195</v>
+        <v>210</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2709,7 +2855,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2771,10 +2917,10 @@
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="1"/>
@@ -2806,16 +2952,16 @@
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="6" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -2831,13 +2977,13 @@
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -2853,13 +2999,13 @@
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -2875,13 +3021,13 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -2897,13 +3043,13 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -2918,7 +3064,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2972,7 +3118,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2994,7 +3140,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>9</v>
@@ -3015,7 +3161,7 @@
       <c r="B4" s="6"/>
       <c r="C4" s="1"/>
       <c r="D4" s="6" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>12</v>
@@ -3034,13 +3180,13 @@
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -3056,10 +3202,10 @@
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="1"/>
@@ -3076,13 +3222,13 @@
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -3097,7 +3243,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -3113,7 +3259,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3142,7 +3288,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -3177,23 +3323,23 @@
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E6" s="2"/>
     </row>
@@ -3207,7 +3353,7 @@
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1"/>
       <c r="B8" s="6" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>17</v>
@@ -3216,33 +3362,33 @@
         <v>18</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3250,7 +3396,7 @@
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="E11" s="2"/>
     </row>
@@ -3258,26 +3404,26 @@
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E13" s="2"/>
     </row>
@@ -3291,7 +3437,7 @@
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1"/>
       <c r="B15" s="6" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>17</v>
@@ -3300,17 +3446,17 @@
         <v>18</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E16" s="2"/>
     </row>
@@ -3324,7 +3470,7 @@
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1"/>
       <c r="B18" s="6" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>17</v>
@@ -3333,7 +3479,7 @@
         <v>18</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3346,39 +3492,39 @@
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1"/>
       <c r="B20" s="6" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1"/>
       <c r="B21" s="6"/>
       <c r="C21" s="1" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1"/>
       <c r="B22" s="6"/>
       <c r="C22" s="1" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E22" s="2"/>
     </row>
@@ -3392,13 +3538,13 @@
         <v>18</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -3444,18 +3590,18 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>9</v>
@@ -3467,35 +3613,35 @@
         <v>11</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D5" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E5" s="8" t="n">
+        <v>105</v>
+      </c>
+      <c r="E5" s="9" t="n">
         <v>1500</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C6" s="6"/>
       <c r="D6" s="6" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3548,7 +3694,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3564,13 +3710,13 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3578,7 +3724,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -3599,8 +3745,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="9" width="12.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="9" width="10.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="12.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="10.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="45.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.74"/>
@@ -3608,16 +3754,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="B1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="10" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>9</v>
@@ -3625,43 +3771,43 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="0" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="1" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="1"/>
       <c r="D6" s="6" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="1"/>
       <c r="D7" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="E7" s="10"/>
+        <v>119</v>
+      </c>
+      <c r="E7" s="11"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="1"/>
@@ -3669,11 +3815,11 @@
       <c r="E8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="9" t="s">
-        <v>32</v>
+      <c r="B9" s="10" t="s">
+        <v>37</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>9</v>
@@ -3681,54 +3827,54 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>18</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>18</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D14" s="6" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -3744,7 +3890,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3772,7 +3918,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -3782,10 +3928,10 @@
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="6" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>9</v>
@@ -3800,17 +3946,17 @@
         <v>11</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E5" s="2"/>
     </row>
@@ -3819,7 +3965,7 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="E6" s="2"/>
     </row>
@@ -3827,10 +3973,10 @@
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>114</v>
+        <v>130</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="E7" s="2"/>
     </row>
@@ -3839,7 +3985,7 @@
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="E8" s="2"/>
     </row>
@@ -3847,10 +3993,10 @@
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>114</v>
+        <v>130</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>115</v>
+        <v>131</v>
       </c>
       <c r="E9" s="2"/>
     </row>
@@ -3858,13 +4004,13 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>114</v>
+        <v>130</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>18</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3897,7 +4043,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -3941,7 +4087,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -3951,10 +4097,10 @@
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="6" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>9</v>
@@ -3969,17 +4115,17 @@
         <v>11</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E5" s="2"/>
     </row>
@@ -3987,10 +4133,10 @@
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="E6" s="2"/>
     </row>
@@ -3998,7 +4144,7 @@
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>18</v>
@@ -4011,10 +4157,10 @@
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E8" s="2"/>
     </row>
@@ -4022,7 +4168,7 @@
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>18</v>
@@ -4035,10 +4181,10 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="E10" s="2"/>
     </row>
@@ -4046,7 +4192,7 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>18</v>
@@ -4099,7 +4245,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>